<commit_message>
Ticket [1] - Dynamic value for the graph
</commit_message>
<xml_diff>
--- a/webapp/admin/import/trueinsight_school.xlsx
+++ b/webapp/admin/import/trueinsight_school.xlsx
@@ -1,31 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20486" windowHeight="7458"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$18</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="14">
   <si>
     <t>A</t>
   </si>
   <si>
-    <t>A,B</t>
-  </si>
-  <si>
     <t>JP Nagar Center</t>
   </si>
   <si>
@@ -59,22 +56,16 @@
     <t>UKG</t>
   </si>
   <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>LKG</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> LKG</t>
+    <t>Rajajinagar Center</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -112,9 +103,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -208,23 +200,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -260,23 +235,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -453,60 +411,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>1</v>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -514,125 +472,236 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" t="s">
-        <v>15</v>
+      <c r="C8" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" t="s">
-        <v>15</v>
+      <c r="C11" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
-        <v>15</v>
+      <c r="C13" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="C15" t="s">
-        <v>1</v>
+      <c r="C16" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A15"/>
+  <autoFilter ref="A1:A18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -642,7 +711,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>